<commit_message>
Fixed a issue removing/adding sheets
Fixed a issue removing/adding sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/files/OrangeHRMUserRoles.xlsx
+++ b/src/test/resources/files/OrangeHRMUserRoles.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spot\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\eclipse-workspace\orangehrm\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465DA5D4-D332-439C-AA1C-413DA54069FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97648FD0-94BF-4F53-9509-E89D5C93C846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4590" yWindow="4590" windowWidth="43200" windowHeight="23985" xr2:uid="{A2E5FF97-6E86-42DB-8CA9-8BFCAE213B90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ESS_users" r:id="rId6" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,15 +33,118 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
   <si>
     <t>ESS</t>
+  </si>
+  <si>
+    <t>Aaliyah.Haq</t>
+  </si>
+  <si>
+    <t>Aatmaram</t>
+  </si>
+  <si>
+    <t>Alice.Duval</t>
+  </si>
+  <si>
+    <t>Anthony.Nolan</t>
+  </si>
+  <si>
+    <t>Aravind</t>
+  </si>
+  <si>
+    <t>azq@gmail.com</t>
+  </si>
+  <si>
+    <t>Cassidy.Hope</t>
+  </si>
+  <si>
+    <t>catelusCuParulCret</t>
+  </si>
+  <si>
+    <t>Cecil.Bonaparte</t>
+  </si>
+  <si>
+    <t>Charlie.Carter</t>
+  </si>
+  <si>
+    <t>Chenzira.Chuki</t>
+  </si>
+  <si>
+    <t>David.Morris</t>
+  </si>
+  <si>
+    <t>Ehioze.Ebo</t>
+  </si>
+  <si>
+    <t>Fiona.Grace</t>
+  </si>
+  <si>
+    <t>Garry.White</t>
+  </si>
+  <si>
+    <t>Goutam.Ganesh</t>
+  </si>
+  <si>
+    <t>Jacqueline.White</t>
+  </si>
+  <si>
+    <t>Jadine.Jackie</t>
+  </si>
+  <si>
+    <t>Jasmine.Morgan</t>
+  </si>
+  <si>
+    <t>Joe.Root</t>
+  </si>
+  <si>
+    <t>Jordan.Mathews</t>
+  </si>
+  <si>
+    <t>Kevin.Mathews</t>
+  </si>
+  <si>
+    <t>Kiyara.Hu</t>
+  </si>
+  <si>
+    <t>Lisa.Andrews</t>
+  </si>
+  <si>
+    <t>Luke.Wright</t>
+  </si>
+  <si>
+    <t>Maggie.Manning</t>
+  </si>
+  <si>
+    <t>manali28</t>
+  </si>
+  <si>
+    <t>Melan.Peiris</t>
+  </si>
+  <si>
+    <t>Nathan.Elliot</t>
+  </si>
+  <si>
+    <t>Nina.Patel</t>
+  </si>
+  <si>
+    <t>Rebecca.Harmony</t>
+  </si>
+  <si>
+    <t>Russel.Hamilton</t>
+  </si>
+  <si>
+    <t>Sania.Shaheen</t>
+  </si>
+  <si>
+    <t>Sara.Tencrady</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D206E51-75D9-4B6A-84D6-2506E3E87313}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -400,4 +506,187 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>